<commit_message>
Match conventions and units with simulink
</commit_message>
<xml_diff>
--- a/Config_Opt.xlsx
+++ b/Config_Opt.xlsx
@@ -8,17 +8,28 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\szata\Codes\StoriesTeams\DispatchOptimisation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{893ABE8E-1B38-40CF-9FFD-2BB52B085946}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63A89F5B-E68B-4222-A86B-73F8D63BDA65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -43,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="32">
   <si>
     <t>None</t>
   </si>
@@ -127,13 +138,25 @@
   </si>
   <si>
     <t>Opt_Value</t>
+  </si>
+  <si>
+    <t>CI_th</t>
+  </si>
+  <si>
+    <t>CI_el</t>
+  </si>
+  <si>
+    <t>w</t>
+  </si>
+  <si>
+    <t>CO2Price</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -142,24 +165,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -174,11 +197,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -473,10 +497,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D36"/>
+  <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -778,7 +802,7 @@
         <v>10</v>
       </c>
       <c r="D21" s="1">
-        <v>185</v>
+        <v>286.25</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -862,7 +886,7 @@
         <v>16</v>
       </c>
       <c r="D27" s="1">
-        <v>1E-3</v>
+        <v>1.1000000000000001E-3</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
@@ -876,7 +900,7 @@
         <v>10</v>
       </c>
       <c r="D28" s="1">
-        <v>150</v>
+        <v>205</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
@@ -960,7 +984,7 @@
         <v>16</v>
       </c>
       <c r="D34" s="1">
-        <v>3.0000000000000001E-3</v>
+        <v>6.1500000000000001E-3</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
@@ -991,8 +1015,64 @@
         <v>0.38</v>
       </c>
     </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>0</v>
+      </c>
+      <c r="B37" t="s">
+        <v>4</v>
+      </c>
+      <c r="C37" t="s">
+        <v>28</v>
+      </c>
+      <c r="D37" s="1">
+        <v>0.20200000000000001</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>0</v>
+      </c>
+      <c r="B38" t="s">
+        <v>4</v>
+      </c>
+      <c r="C38" t="s">
+        <v>29</v>
+      </c>
+      <c r="D38" s="1">
+        <v>0.35399999999999998</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>0</v>
+      </c>
+      <c r="B39" t="s">
+        <v>4</v>
+      </c>
+      <c r="C39" t="s">
+        <v>30</v>
+      </c>
+      <c r="D39" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>0</v>
+      </c>
+      <c r="B40" t="s">
+        <v>4</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D40" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>